<commit_message>
Guru Mapel Import Feature Enhanced
</commit_message>
<xml_diff>
--- a/public/templates/ImporGuruMapel.xlsx
+++ b/public/templates/ImporGuruMapel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Project\Laravel\AgendaKBM\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9EEA94-3927-4F0B-BABB-3C8940A84AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED394E-779B-41F5-8D9B-ECFECAA7DB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9992942B-78AE-47AE-AB12-617A079D18F5}"/>
   </bookViews>
@@ -159,19 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD466F9-3602-439F-8BAB-086A6D24FD04}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,39 +516,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>86</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>72</v>
-      </c>
-      <c r="B4" s="4">
-        <v>54</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>72</v>
-      </c>
-      <c r="B5" s="4">
-        <v>60</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>